<commit_message>
Refactored to be more in line with other Diageo projects
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOCO_SAND/Data/Diageo Colombia - Kpi Bank - 29102018.xlsx
+++ b/Projects/DIAGEOCO_SAND/Data/Diageo Colombia - Kpi Bank - 29102018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kick off KPI's" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,6 +33,7 @@
     <definedName function="false" hidden="false" name="YN" vbProcedure="false">tbl_YN[Yes / No]</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Kick off KPI''s'!$A$1:$J$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Kick off KPI''s'!$A$1:$J$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Kick off KPI''s'!$A$1:$J$19</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Channel" vbProcedure="false">[1]!tbl_Channel[channel]</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Diageo_Brands" vbProcedure="false">[1]!tbl_Diageo_Brands[diageo brands]</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Distance" vbProcedure="false">[1]!tbl_Distance[distance]</definedName>
@@ -700,13 +701,13 @@
     <t xml:space="preserve">Tested Product Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Tested Product ID</t>
+    <t xml:space="preserve">Tested SKU2</t>
   </si>
   <si>
     <t xml:space="preserve">Anchor Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Anchor Product ID</t>
+    <t xml:space="preserve">Anchor SKU2</t>
   </si>
   <si>
     <t xml:space="preserve">Above Allowed? </t>
@@ -2335,7 +2336,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2454,13 +2455,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>750240</xdr:colOff>
       <xdr:row>215</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>773280</xdr:colOff>
+      <xdr:colOff>772920</xdr:colOff>
       <xdr:row>239</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2474,7 +2475,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="750240" y="41433840"/>
-          <a:ext cx="6947640" cy="4590360"/>
+          <a:ext cx="6994800" cy="4590000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2500,9 +2501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1873080</xdr:colOff>
+      <xdr:colOff>1872720</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>190800</xdr:rowOff>
+      <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2516,7 +2517,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4320"/>
-          <a:ext cx="1873080" cy="376920"/>
+          <a:ext cx="1872720" cy="376560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2537,9 +2538,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>86400</xdr:colOff>
+      <xdr:colOff>86040</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2553,7 +2554,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2112480" y="20880"/>
-          <a:ext cx="1202760" cy="342720"/>
+          <a:ext cx="1230840" cy="342360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2624,9 +2625,9 @@
     <tableColumn id="3" name="Template Group"/>
     <tableColumn id="4" name="Tested Type"/>
     <tableColumn id="5" name="Tested Product Name"/>
-    <tableColumn id="6" name="Tested Product ID"/>
+    <tableColumn id="6" name="Tested SKU2"/>
     <tableColumn id="7" name="Anchor Type"/>
-    <tableColumn id="8" name="Anchor Product ID"/>
+    <tableColumn id="8" name="Anchor SKU2"/>
     <tableColumn id="9" name="Above Allowed? "/>
     <tableColumn id="10" name="Up to (above) distance (by shelves) "/>
     <tableColumn id="11" name="Below Allowed?"/>
@@ -2793,47 +2794,47 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="45.0971659919028"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="43.0607287449393"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="43.4898785425101"/>
     <col collapsed="false" hidden="false" max="254" min="11" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="255" min="255" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="256" min="256" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="256" min="256" style="1" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="257" min="257" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="259" min="259" style="1" width="45.0971659919028"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="1" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="262" min="261" style="1" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="263" min="263" style="1" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="264" min="264" style="1" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="259" min="259" style="1" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="1" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="262" min="261" style="1" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="263" min="263" style="1" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="264" min="264" style="1" width="34.7085020242915"/>
     <col collapsed="false" hidden="false" max="510" min="265" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="511" min="511" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="512" min="512" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="512" min="512" style="1" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="513" min="513" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="515" min="515" style="1" width="45.0971659919028"/>
-    <col collapsed="false" hidden="false" max="516" min="516" style="1" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="518" min="517" style="1" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="519" min="519" style="1" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="520" min="520" style="1" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="515" min="515" style="1" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="516" min="516" style="1" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="518" min="517" style="1" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="519" min="519" style="1" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="520" min="520" style="1" width="34.7085020242915"/>
     <col collapsed="false" hidden="false" max="766" min="521" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="767" min="767" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="768" min="768" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="768" min="768" style="1" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="769" min="769" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="771" min="771" style="1" width="45.0971659919028"/>
-    <col collapsed="false" hidden="false" max="772" min="772" style="1" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="774" min="773" style="1" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="775" min="775" style="1" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="776" min="776" style="1" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="771" min="771" style="1" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="772" min="772" style="1" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="774" min="773" style="1" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="775" min="775" style="1" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="776" min="776" style="1" width="34.7085020242915"/>
     <col collapsed="false" hidden="false" max="1022" min="777" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="15.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3420,74 +3421,74 @@
   </sheetPr>
   <dimension ref="A2:P213"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.4858299595142"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.2388663967611"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.0202429149798"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="255" min="17" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="256" min="256" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="257" min="257" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="257" min="257" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="259" min="259" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="262" min="262" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="262" min="262" style="0" width="38.9919028340081"/>
     <col collapsed="false" hidden="false" max="263" min="263" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="264" min="264" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="265" min="265" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="264" min="264" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="265" min="265" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="266" min="266" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="267" min="267" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="268" min="268" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="269" min="269" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="270" min="270" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="269" min="269" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="270" min="270" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="511" min="271" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="512" min="512" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="513" min="513" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="513" min="513" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="515" min="515" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="516" min="516" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="517" min="517" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="518" min="518" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="516" min="516" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="517" min="517" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="518" min="518" style="0" width="38.9919028340081"/>
     <col collapsed="false" hidden="false" max="519" min="519" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="520" min="520" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="521" min="521" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="520" min="520" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="521" min="521" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="522" min="522" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="523" min="523" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="524" min="524" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="525" min="525" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="526" min="526" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="525" min="525" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="526" min="526" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="767" min="527" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="768" min="768" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="769" min="769" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="769" min="769" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="771" min="771" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="772" min="772" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="773" min="773" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="774" min="774" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="772" min="772" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="773" min="773" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="774" min="774" style="0" width="38.9919028340081"/>
     <col collapsed="false" hidden="false" max="775" min="775" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="776" min="776" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="777" min="777" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="776" min="776" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="777" min="777" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="778" min="778" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="779" min="779" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="780" min="780" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="781" min="781" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="782" min="782" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="781" min="781" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="782" min="782" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="1023" min="783" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="3"/>
   </cols>
@@ -3513,7 +3514,7 @@
       </c>
       <c r="P4" s="79"/>
     </row>
-    <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="80" t="s">
         <v>99</v>
       </c>
@@ -14038,57 +14039,57 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.0283400809717"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="253" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="254" min="254" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="255" min="255" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="256" min="256" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="255" min="255" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="256" min="256" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="257" min="257" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="259" min="259" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="259" min="259" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="262" min="262" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="263" min="263" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="264" min="264" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="265" min="265" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="264" min="264" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="265" min="265" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="509" min="266" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="510" min="510" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="511" min="511" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="512" min="512" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="511" min="511" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="512" min="512" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="513" min="513" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="515" min="515" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="516" min="516" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="517" min="517" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="515" min="515" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="516" min="516" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="517" min="517" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="518" min="518" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="519" min="519" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="520" min="520" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="521" min="521" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="520" min="520" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="521" min="521" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="765" min="522" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="766" min="766" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="767" min="767" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="768" min="768" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="767" min="767" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="768" min="768" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="769" min="769" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="771" min="771" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="772" min="772" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="773" min="773" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="771" min="771" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="772" min="772" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="773" min="773" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="774" min="774" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="775" min="775" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="776" min="776" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="777" min="777" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="776" min="776" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="777" min="777" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="1021" min="778" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1022" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="1023" min="1023" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="1023" min="1023" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="73.2712550607288"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14501,7 +14502,7 @@
   </sheetPr>
   <dimension ref="B1:E11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -14509,56 +14510,56 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="251" min="8" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="252" min="252" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="253" min="253" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="254" min="254" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="253" min="253" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="254" min="254" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="255" min="255" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="256" min="256" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="257" min="257" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="259" min="259" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="256" min="256" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="257" min="257" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="259" min="259" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="260" min="260" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="261" min="261" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="262" min="262" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="263" min="263" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="262" min="262" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="263" min="263" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="507" min="264" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="508" min="508" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="509" min="509" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="510" min="510" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="509" min="509" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="510" min="510" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="511" min="511" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="512" min="512" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="513" min="513" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="515" min="515" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="512" min="512" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="513" min="513" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="515" min="515" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="516" min="516" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="517" min="517" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="518" min="518" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="519" min="519" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="518" min="518" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="519" min="519" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="763" min="520" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="764" min="764" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="765" min="765" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="766" min="766" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="765" min="765" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="766" min="766" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="767" min="767" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="768" min="768" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="769" min="769" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="771" min="771" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="768" min="768" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="769" min="769" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="771" min="771" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="772" min="772" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="773" min="773" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="774" min="774" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="775" min="775" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="774" min="774" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="775" min="775" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="1019" min="776" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1020" min="1020" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="1021" min="1021" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="1022" min="1022" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="1021" min="1021" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1022" min="1022" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="1023" min="1023" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="13.1740890688259"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14702,53 +14703,53 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.53441295546559"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="255" min="12" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="256" min="256" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="257" min="257" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="257" min="257" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="259" min="259" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="261" min="261" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="262" min="262" style="0" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="263" min="263" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="264" min="264" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="262" min="262" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="263" min="263" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="264" min="264" style="0" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="265" min="265" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="266" min="266" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="267" min="267" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="266" min="266" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="267" min="267" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="511" min="268" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="512" min="512" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="513" min="513" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="513" min="513" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="515" min="515" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="516" min="516" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="516" min="516" style="0" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="517" min="517" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="518" min="518" style="0" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="519" min="519" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="520" min="520" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="518" min="518" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="519" min="519" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="520" min="520" style="0" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="521" min="521" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="522" min="522" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="523" min="523" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="522" min="522" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="523" min="523" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="767" min="524" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="768" min="768" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="769" min="769" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="72.6275303643725"/>
+    <col collapsed="false" hidden="false" max="769" min="769" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="73.2712550607288"/>
     <col collapsed="false" hidden="false" max="771" min="771" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="772" min="772" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="772" min="772" style="0" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="773" min="773" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="774" min="774" style="0" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="775" min="775" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="776" min="776" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="774" min="774" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="775" min="775" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="776" min="776" style="0" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="777" min="777" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="778" min="778" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="779" min="779" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="778" min="778" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="779" min="779" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="1023" min="780" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="3"/>
   </cols>
@@ -14869,10 +14870,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.9514170040486"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.67611336032389"/>
   </cols>
   <sheetData>
@@ -15021,40 +15022,40 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="54.2024291497976"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="54.6315789473684"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="259" min="13" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="260" min="260" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="262" min="262" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="263" min="263" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="262" min="262" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="263" min="263" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="264" min="264" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="265" min="265" style="0" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="266" min="266" style="0" width="54.2024291497976"/>
+    <col collapsed="false" hidden="false" max="266" min="266" style="0" width="54.6315789473684"/>
     <col collapsed="false" hidden="false" max="515" min="267" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="516" min="516" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="517" min="517" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="518" min="518" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="519" min="519" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="517" min="517" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="518" min="518" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="519" min="519" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="520" min="520" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="521" min="521" style="0" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="522" min="522" style="0" width="54.2024291497976"/>
+    <col collapsed="false" hidden="false" max="522" min="522" style="0" width="54.6315789473684"/>
     <col collapsed="false" hidden="false" max="771" min="523" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="772" min="772" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="773" min="773" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="774" min="774" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="775" min="775" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="773" min="773" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="774" min="774" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="775" min="775" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="776" min="776" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="777" min="777" style="0" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="778" min="778" style="0" width="54.2024291497976"/>
+    <col collapsed="false" hidden="false" max="778" min="778" style="0" width="54.6315789473684"/>
     <col collapsed="false" hidden="false" max="1025" min="779" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>